<commit_message>
documentos sobre presentacion de resultados de reunion de monitoreo
</commit_message>
<xml_diff>
--- a/Proyectos/2015/Métricas y monitoreo/Acciones_correctivas_2015.xlsx
+++ b/Proyectos/2015/Métricas y monitoreo/Acciones_correctivas_2015.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>Se decide esperar hasta dentro de 3 meses mínimo para poder decidir si se requiere realizar acciones correctivas debido a que es una implementación nueva al proceso y no se puede tomar correcciones con resultados tan espontaneos</t>
+  </si>
+  <si>
+    <t>Tiempo sobre elevados en actividades y nulos en otras</t>
+  </si>
+  <si>
+    <t>Hablar sobre poner omentarios de tiempo real en caso de olvidar detener el tracking</t>
+  </si>
+  <si>
+    <t>Abierto</t>
+  </si>
+  <si>
+    <t>Multiples proyectos sin hito de cierre</t>
+  </si>
+  <si>
+    <t>Hacer el hito de cierre con una enuesta de satisfaccion</t>
   </si>
 </sst>
 </file>
@@ -349,8 +364,8 @@
   </sheetPr>
   <dimension ref="1:26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -558,31 +573,55 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>42377</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <v>42685</v>
+      </c>
       <c r="H8" s="10"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="10"/>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>42377</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <v>42685</v>
+      </c>
       <c r="H9" s="10"/>
-      <c r="I9" s="8"/>
+      <c r="I9" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>

</xml_diff>